<commit_message>
empty file still no passing through code
</commit_message>
<xml_diff>
--- a/R_VisualizeOldMethods.xlsx
+++ b/R_VisualizeOldMethods.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="R_VisualizeOldMethods" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4566" uniqueCount="1559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4571" uniqueCount="1559">
   <si>
     <t>DVDRef</t>
   </si>
@@ -5573,8 +5573,8 @@
   <dimension ref="A1:O1528"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O41" sqref="O41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5961,6 +5961,21 @@
       <c r="I10" s="3">
         <v>0</v>
       </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
@@ -5990,6 +6005,21 @@
       <c r="I11" s="3">
         <v>1</v>
       </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
@@ -6018,6 +6048,21 @@
       </c>
       <c r="I12" s="3">
         <v>5</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
all warningzz listed get color of a cell
</commit_message>
<xml_diff>
--- a/R_VisualizeOldMethods.xlsx
+++ b/R_VisualizeOldMethods.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="348" windowWidth="22692" windowHeight="8148"/>
+    <workbookView xWindow="288" yWindow="408" windowWidth="22692" windowHeight="8088"/>
   </bookViews>
   <sheets>
     <sheet name="R_VisualizeOldMethods" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4571" uniqueCount="1559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4685" uniqueCount="1563">
   <si>
     <t>DVDRef</t>
   </si>
@@ -4691,6 +4691,18 @@
   </si>
   <si>
     <t>cop</t>
+  </si>
+  <si>
+    <t>comments describe meaning blue and grey: grey = out no feed, blue = out feed</t>
+  </si>
+  <si>
+    <t>new type of blue color</t>
+  </si>
+  <si>
+    <t>long O blue mistake ?? Should be grey ??</t>
+  </si>
+  <si>
+    <t>some G in grey !!! Should be O ???</t>
   </si>
 </sst>
 </file>
@@ -4834,7 +4846,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5032,6 +5044,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -5193,7 +5211,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5205,6 +5223,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5573,8 +5594,8 @@
   <dimension ref="A1:O1528"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
+      <pane ySplit="1" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I694" sqref="I694"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5590,7 +5611,8 @@
     <col min="9" max="9" width="7.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.88671875" style="4"/>
     <col min="12" max="12" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="65.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
@@ -5845,6 +5867,21 @@
       <c r="I6" s="3">
         <v>0</v>
       </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
@@ -5874,6 +5911,21 @@
       <c r="I7" s="3">
         <v>1</v>
       </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
@@ -5903,6 +5955,21 @@
       <c r="I8" s="3">
         <v>18</v>
       </c>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
@@ -5931,6 +5998,21 @@
       </c>
       <c r="I9" s="3">
         <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -6093,6 +6175,21 @@
       <c r="I13" s="3">
         <v>0</v>
       </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
@@ -6122,6 +6219,21 @@
       <c r="I14" s="3">
         <v>1</v>
       </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -6151,6 +6263,21 @@
       <c r="I15" s="3">
         <v>3</v>
       </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
@@ -6180,8 +6307,23 @@
       <c r="I16" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>18</v>
       </c>
@@ -6209,8 +6351,23 @@
       <c r="I17" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>19</v>
       </c>
@@ -6238,8 +6395,23 @@
       <c r="I18" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>1</v>
+      </c>
+      <c r="L18" s="4">
+        <v>1</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>21</v>
       </c>
@@ -6267,8 +6439,23 @@
       <c r="I19" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4">
+        <v>1</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>22</v>
       </c>
@@ -6296,8 +6483,23 @@
       <c r="I20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>23</v>
       </c>
@@ -6325,8 +6527,23 @@
       <c r="I21" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
+      </c>
+      <c r="L21" s="4">
+        <v>1</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>25</v>
       </c>
@@ -6354,8 +6571,23 @@
       <c r="I22" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4">
+        <v>1</v>
+      </c>
+      <c r="M22" s="4">
+        <v>1</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>26</v>
       </c>
@@ -6383,8 +6615,23 @@
       <c r="I23" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23" s="4">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <v>1</v>
+      </c>
+      <c r="L23" s="4">
+        <v>1</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>27</v>
       </c>
@@ -6412,8 +6659,23 @@
       <c r="I24" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="4">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
+        <v>1</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>28</v>
       </c>
@@ -6441,8 +6703,23 @@
       <c r="I25" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4">
+        <v>1</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>29</v>
       </c>
@@ -6470,8 +6747,23 @@
       <c r="I26" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>30</v>
       </c>
@@ -6499,8 +6791,23 @@
       <c r="I27" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J27" s="4">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4">
+        <v>1</v>
+      </c>
+      <c r="L27" s="4">
+        <v>1</v>
+      </c>
+      <c r="M27" s="4">
+        <v>0</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>33</v>
       </c>
@@ -6528,8 +6835,23 @@
       <c r="I28" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28" s="4">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4">
+        <v>1</v>
+      </c>
+      <c r="L28" s="4">
+        <v>1</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>34</v>
       </c>
@@ -6557,8 +6879,23 @@
       <c r="I29" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J29" s="4">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <v>1</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>36</v>
       </c>
@@ -6586,8 +6923,23 @@
       <c r="I30" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J30" s="4">
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>37</v>
       </c>
@@ -6615,8 +6967,26 @@
       <c r="I31" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J31" s="4">
+        <v>1</v>
+      </c>
+      <c r="K31" s="4">
+        <v>1</v>
+      </c>
+      <c r="L31" s="4">
+        <v>1</v>
+      </c>
+      <c r="M31" s="4">
+        <v>1</v>
+      </c>
+      <c r="N31" s="4">
+        <v>1</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>38</v>
       </c>
@@ -6643,6 +7013,21 @@
       </c>
       <c r="I32" s="3">
         <v>1</v>
+      </c>
+      <c r="J32" s="4">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4">
+        <v>1</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -6673,6 +7058,21 @@
       <c r="I33" s="3">
         <v>1</v>
       </c>
+      <c r="J33" s="4">
+        <v>0</v>
+      </c>
+      <c r="K33" s="4">
+        <v>1</v>
+      </c>
+      <c r="L33" s="4">
+        <v>1</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
@@ -7191,6 +7591,21 @@
       <c r="I46" s="3">
         <v>0</v>
       </c>
+      <c r="J46" s="4">
+        <v>0</v>
+      </c>
+      <c r="K46" s="4">
+        <v>0</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
@@ -7250,7 +7665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>60</v>
       </c>
@@ -7278,8 +7693,23 @@
       <c r="I49" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J49" s="4">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4">
+        <v>1</v>
+      </c>
+      <c r="L49" s="4">
+        <v>1</v>
+      </c>
+      <c r="M49" s="4">
+        <v>0</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>61</v>
       </c>
@@ -7307,8 +7737,23 @@
       <c r="I50" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J50" s="4">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4">
+        <v>0</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>62</v>
       </c>
@@ -7336,8 +7781,23 @@
       <c r="I51" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51" s="4">
+        <v>0</v>
+      </c>
+      <c r="K51" s="4">
+        <v>1</v>
+      </c>
+      <c r="L51" s="4">
+        <v>1</v>
+      </c>
+      <c r="M51" s="4">
+        <v>0</v>
+      </c>
+      <c r="N51" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>63</v>
       </c>
@@ -7366,7 +7826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>65</v>
       </c>
@@ -7395,7 +7855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>66</v>
       </c>
@@ -7424,7 +7884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>67</v>
       </c>
@@ -7453,7 +7913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>68</v>
       </c>
@@ -7481,8 +7941,23 @@
       <c r="I56" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J56" s="4">
+        <v>0</v>
+      </c>
+      <c r="K56" s="4">
+        <v>0</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N56" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>69</v>
       </c>
@@ -7510,8 +7985,23 @@
       <c r="I57" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J57" s="4">
+        <v>0</v>
+      </c>
+      <c r="K57" s="4">
+        <v>1</v>
+      </c>
+      <c r="L57" s="4">
+        <v>1</v>
+      </c>
+      <c r="M57" s="4">
+        <v>0</v>
+      </c>
+      <c r="N57" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>70</v>
       </c>
@@ -7539,8 +8029,23 @@
       <c r="I58" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J58" s="4">
+        <v>0</v>
+      </c>
+      <c r="K58" s="4">
+        <v>0</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>71</v>
       </c>
@@ -7569,7 +8074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>72</v>
       </c>
@@ -7597,8 +8102,23 @@
       <c r="I60" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J60" s="4">
+        <v>0</v>
+      </c>
+      <c r="K60" s="4">
+        <v>1</v>
+      </c>
+      <c r="L60" s="4">
+        <v>1</v>
+      </c>
+      <c r="M60" s="4">
+        <v>0</v>
+      </c>
+      <c r="N60" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>73</v>
       </c>
@@ -7626,8 +8146,23 @@
       <c r="I61" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J61" s="4">
+        <v>0</v>
+      </c>
+      <c r="K61" s="4">
+        <v>1</v>
+      </c>
+      <c r="L61" s="4">
+        <v>1</v>
+      </c>
+      <c r="M61" s="4">
+        <v>0</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>74</v>
       </c>
@@ -7656,7 +8191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>75</v>
       </c>
@@ -7685,7 +8220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>76</v>
       </c>
@@ -7714,7 +8249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>77</v>
       </c>
@@ -7743,7 +8278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>78</v>
       </c>
@@ -7771,8 +8306,23 @@
       <c r="I66" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J66" s="4">
+        <v>0</v>
+      </c>
+      <c r="K66" s="4">
+        <v>0</v>
+      </c>
+      <c r="L66" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M66" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N66" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>79</v>
       </c>
@@ -7800,8 +8350,23 @@
       <c r="I67" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J67" s="4">
+        <v>0</v>
+      </c>
+      <c r="K67" s="4">
+        <v>1</v>
+      </c>
+      <c r="L67" s="4">
+        <v>1</v>
+      </c>
+      <c r="M67" s="4">
+        <v>0</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>80</v>
       </c>
@@ -7829,8 +8394,23 @@
       <c r="I68" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J68" s="4">
+        <v>0</v>
+      </c>
+      <c r="K68" s="4">
+        <v>0</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>81</v>
       </c>
@@ -7858,8 +8438,23 @@
       <c r="I69" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J69" s="4">
+        <v>0</v>
+      </c>
+      <c r="K69" s="4">
+        <v>1</v>
+      </c>
+      <c r="L69" s="4">
+        <v>1</v>
+      </c>
+      <c r="M69" s="4">
+        <v>0</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>82</v>
       </c>
@@ -7887,8 +8482,26 @@
       <c r="I70" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J70" s="4">
+        <v>1</v>
+      </c>
+      <c r="K70" s="4">
+        <v>0</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N70" s="4">
+        <v>0</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>83</v>
       </c>
@@ -7917,7 +8530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>84</v>
       </c>
@@ -7946,7 +8559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>85</v>
       </c>
@@ -7975,7 +8588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>88</v>
       </c>
@@ -8004,7 +8617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>89</v>
       </c>
@@ -8033,7 +8646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>90</v>
       </c>
@@ -8062,7 +8675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>91</v>
       </c>
@@ -8091,7 +8704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>93</v>
       </c>
@@ -8120,7 +8733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>94</v>
       </c>
@@ -8149,7 +8762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>95</v>
       </c>
@@ -16530,7 +17143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A369" s="3">
         <v>386</v>
       </c>
@@ -16559,7 +17172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A370" s="3">
         <v>387</v>
       </c>
@@ -16588,7 +17201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A371" s="3">
         <v>388</v>
       </c>
@@ -16616,8 +17229,23 @@
       <c r="I371" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J371" s="4">
+        <v>0</v>
+      </c>
+      <c r="K371" s="4">
+        <v>0</v>
+      </c>
+      <c r="L371" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M371" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N371" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="372" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A372" s="3">
         <v>389</v>
       </c>
@@ -16646,7 +17274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A373" s="3">
         <v>390</v>
       </c>
@@ -16675,7 +17303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A374" s="3">
         <v>391</v>
       </c>
@@ -16704,7 +17332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="375" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A375" s="3">
         <v>392</v>
       </c>
@@ -16733,7 +17361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A376" s="3">
         <v>393</v>
       </c>
@@ -16762,7 +17390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A377" s="3">
         <v>394</v>
       </c>
@@ -16791,7 +17419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A378" s="3">
         <v>395</v>
       </c>
@@ -16820,7 +17448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A379" s="3">
         <v>396</v>
       </c>
@@ -16849,7 +17477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A380" s="3">
         <v>397</v>
       </c>
@@ -16878,7 +17506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A381" s="3">
         <v>398</v>
       </c>
@@ -16907,7 +17535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A382" s="3">
         <v>399</v>
       </c>
@@ -16936,7 +17564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A383" s="3">
         <v>400</v>
       </c>
@@ -16965,7 +17593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A384" s="3">
         <v>401</v>
       </c>
@@ -17502,8 +18130,23 @@
       <c r="I400" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J400" s="4">
+        <v>0</v>
+      </c>
+      <c r="K400" s="4">
+        <v>0</v>
+      </c>
+      <c r="L400" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M400" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N400" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="401" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A401" s="3">
         <v>419</v>
       </c>
@@ -17532,7 +18175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A402" s="3">
         <v>420</v>
       </c>
@@ -17560,8 +18203,23 @@
       <c r="I402" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J402" s="4">
+        <v>0</v>
+      </c>
+      <c r="K402" s="4">
+        <v>1</v>
+      </c>
+      <c r="L402" s="4">
+        <v>1</v>
+      </c>
+      <c r="M402" s="4">
+        <v>1</v>
+      </c>
+      <c r="N402" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="403" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A403" s="3">
         <v>421</v>
       </c>
@@ -17590,7 +18248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A404" s="3">
         <v>422</v>
       </c>
@@ -17619,7 +18277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A405" s="3">
         <v>423</v>
       </c>
@@ -17648,7 +18306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A406" s="3">
         <v>424</v>
       </c>
@@ -17677,7 +18335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A407" s="3">
         <v>425</v>
       </c>
@@ -17706,7 +18364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A408" s="3">
         <v>426</v>
       </c>
@@ -17735,7 +18393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A409" s="3">
         <v>427</v>
       </c>
@@ -17764,7 +18422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A410" s="3">
         <v>428</v>
       </c>
@@ -17793,7 +18451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A411" s="3">
         <v>429</v>
       </c>
@@ -17822,7 +18480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A412" s="3">
         <v>430</v>
       </c>
@@ -17851,7 +18509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A413" s="3">
         <v>431</v>
       </c>
@@ -17880,7 +18538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A414" s="3">
         <v>432</v>
       </c>
@@ -17909,7 +18567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="415" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A415" s="3">
         <v>433</v>
       </c>
@@ -17938,7 +18596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A416" s="3">
         <v>434</v>
       </c>
@@ -17967,7 +18625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A417" s="3">
         <v>435</v>
       </c>
@@ -17995,8 +18653,23 @@
       <c r="I417" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="418" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J417" s="4">
+        <v>0</v>
+      </c>
+      <c r="K417" s="4">
+        <v>1</v>
+      </c>
+      <c r="L417" s="4">
+        <v>1</v>
+      </c>
+      <c r="M417" s="4">
+        <v>1</v>
+      </c>
+      <c r="N417" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="418" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A418" s="3">
         <v>436</v>
       </c>
@@ -18025,7 +18698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="419" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A419" s="3">
         <v>437</v>
       </c>
@@ -18054,7 +18727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="420" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A420" s="3">
         <v>438</v>
       </c>
@@ -18083,7 +18756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A421" s="3">
         <v>439</v>
       </c>
@@ -18112,7 +18785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="422" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A422" s="3">
         <v>440</v>
       </c>
@@ -18141,7 +18814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="423" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A423" s="3">
         <v>441</v>
       </c>
@@ -18170,7 +18843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A424" s="3">
         <v>442</v>
       </c>
@@ -18199,7 +18872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A425" s="3">
         <v>443</v>
       </c>
@@ -18228,7 +18901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A426" s="3">
         <v>444</v>
       </c>
@@ -18257,7 +18930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="427" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A427" s="3">
         <v>445</v>
       </c>
@@ -18286,7 +18959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A428" s="3">
         <v>446</v>
       </c>
@@ -18315,7 +18988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="429" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A429" s="3">
         <v>447</v>
       </c>
@@ -18344,7 +19017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="430" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A430" s="3">
         <v>448</v>
       </c>
@@ -18373,7 +19046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="431" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A431" s="3">
         <v>449</v>
       </c>
@@ -18402,7 +19075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A432" s="3">
         <v>450</v>
       </c>
@@ -25871,6 +26544,21 @@
       <c r="I671" s="3">
         <v>1</v>
       </c>
+      <c r="J671" s="4">
+        <v>0</v>
+      </c>
+      <c r="K671" s="4">
+        <v>1</v>
+      </c>
+      <c r="L671" s="4">
+        <v>1</v>
+      </c>
+      <c r="M671" s="4">
+        <v>0</v>
+      </c>
+      <c r="N671" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="672" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A672" s="3">
@@ -25901,7 +26589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="673" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="673" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A673" s="3">
         <v>694</v>
       </c>
@@ -25929,8 +26617,23 @@
       <c r="I673" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="674" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J673" s="4">
+        <v>0</v>
+      </c>
+      <c r="K673" s="4">
+        <v>0</v>
+      </c>
+      <c r="L673" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M673" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N673" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="674" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A674" s="3">
         <v>695</v>
       </c>
@@ -25958,8 +26661,23 @@
       <c r="I674" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="675" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J674" s="4">
+        <v>0</v>
+      </c>
+      <c r="K674" s="4">
+        <v>0</v>
+      </c>
+      <c r="L674" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M674" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N674" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="675" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A675" s="3">
         <v>696</v>
       </c>
@@ -25988,7 +26706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="676" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="676" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A676" s="3">
         <v>697</v>
       </c>
@@ -26017,7 +26735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="677" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="677" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A677" s="3">
         <v>698</v>
       </c>
@@ -26046,7 +26764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="678" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="678" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A678" s="3">
         <v>699</v>
       </c>
@@ -26075,7 +26793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="679" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="679" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A679" s="3">
         <v>700</v>
       </c>
@@ -26104,7 +26822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="680" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="680" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A680" s="3">
         <v>701</v>
       </c>
@@ -26132,8 +26850,23 @@
       <c r="I680" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="681" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J680" s="4">
+        <v>0</v>
+      </c>
+      <c r="K680" s="4">
+        <v>0</v>
+      </c>
+      <c r="L680" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M680" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N680" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="681" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A681" s="3">
         <v>702</v>
       </c>
@@ -26161,8 +26894,23 @@
       <c r="I681" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="682" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J681" s="4">
+        <v>0</v>
+      </c>
+      <c r="K681" s="4">
+        <v>0</v>
+      </c>
+      <c r="L681" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M681" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N681" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="682" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A682" s="3">
         <v>703</v>
       </c>
@@ -26190,8 +26938,23 @@
       <c r="I682" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="683" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J682" s="4">
+        <v>0</v>
+      </c>
+      <c r="K682" s="4">
+        <v>1</v>
+      </c>
+      <c r="L682" s="4">
+        <v>1</v>
+      </c>
+      <c r="M682" s="4">
+        <v>0</v>
+      </c>
+      <c r="N682" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="683" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A683" s="3">
         <v>704</v>
       </c>
@@ -26219,8 +26982,23 @@
       <c r="I683" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="684" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J683" s="4">
+        <v>0</v>
+      </c>
+      <c r="K683" s="4">
+        <v>0</v>
+      </c>
+      <c r="L683" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M683" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N683" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="684" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A684" s="3">
         <v>705</v>
       </c>
@@ -26248,8 +27026,23 @@
       <c r="I684" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="685" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J684" s="4">
+        <v>0</v>
+      </c>
+      <c r="K684" s="4">
+        <v>0</v>
+      </c>
+      <c r="L684" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M684" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N684" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="685" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A685" s="3">
         <v>706</v>
       </c>
@@ -26278,7 +27071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="686" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="686" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A686" s="3">
         <v>707</v>
       </c>
@@ -26306,8 +27099,23 @@
       <c r="I686" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="687" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J686" s="4">
+        <v>0</v>
+      </c>
+      <c r="K686" s="4">
+        <v>1</v>
+      </c>
+      <c r="L686" s="4">
+        <v>1</v>
+      </c>
+      <c r="M686" s="4">
+        <v>0</v>
+      </c>
+      <c r="N686" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="687" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A687" s="3">
         <v>708</v>
       </c>
@@ -26336,7 +27144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="688" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="688" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A688" s="3">
         <v>709</v>
       </c>
@@ -26365,7 +27173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="689" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="689" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A689" s="3">
         <v>710</v>
       </c>
@@ -26394,7 +27202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="690" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="690" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A690" s="3">
         <v>711</v>
       </c>
@@ -26423,7 +27231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="691" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="691" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A691" s="3">
         <v>712</v>
       </c>
@@ -26452,7 +27260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="692" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="692" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A692" s="3">
         <v>713</v>
       </c>
@@ -26481,7 +27289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="693" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="693" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A693" s="3">
         <v>714</v>
       </c>
@@ -26510,7 +27318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="694" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="694" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A694" s="3">
         <v>715</v>
       </c>
@@ -26538,8 +27346,23 @@
       <c r="I694" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="695" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J694" s="4">
+        <v>0</v>
+      </c>
+      <c r="K694" s="4">
+        <v>0</v>
+      </c>
+      <c r="L694" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M694" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N694" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="695" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A695" s="3">
         <v>716</v>
       </c>
@@ -26568,7 +27391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="696" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="696" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A696" s="3">
         <v>717</v>
       </c>
@@ -26597,7 +27420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="697" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="697" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A697" s="3">
         <v>718</v>
       </c>
@@ -26625,8 +27448,23 @@
       <c r="I697" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="698" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J697" s="4">
+        <v>0</v>
+      </c>
+      <c r="K697" s="4">
+        <v>0</v>
+      </c>
+      <c r="L697" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M697" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N697" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="698" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A698" s="3">
         <v>719</v>
       </c>
@@ -26654,8 +27492,26 @@
       <c r="I698" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="699" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J698" s="4">
+        <v>0</v>
+      </c>
+      <c r="K698" s="4">
+        <v>0</v>
+      </c>
+      <c r="L698" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M698" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N698" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O698" s="4" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="699" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A699" s="3">
         <v>720</v>
       </c>
@@ -26684,7 +27540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="700" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="700" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A700" s="3">
         <v>721</v>
       </c>
@@ -26713,7 +27569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="701" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="701" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A701" s="3">
         <v>722</v>
       </c>
@@ -26742,7 +27598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="702" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="702" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A702" s="3">
         <v>723</v>
       </c>
@@ -26771,7 +27627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="703" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="703" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A703" s="3">
         <v>724</v>
       </c>
@@ -26800,7 +27656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="704" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="704" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A704" s="3">
         <v>725</v>
       </c>
@@ -27293,7 +28149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="721" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="721" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A721" s="3">
         <v>742</v>
       </c>
@@ -27322,7 +28178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="722" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="722" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A722" s="3">
         <v>743</v>
       </c>
@@ -27351,7 +28207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="723" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="723" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A723" s="3">
         <v>744</v>
       </c>
@@ -27380,7 +28236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="724" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="724" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A724" s="3">
         <v>745</v>
       </c>
@@ -27409,7 +28265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="725" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="725" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A725" s="3">
         <v>746</v>
       </c>
@@ -27438,7 +28294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="726" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="726" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A726" s="3">
         <v>747</v>
       </c>
@@ -27467,7 +28323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="727" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="727" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A727" s="3">
         <v>748</v>
       </c>
@@ -27496,7 +28352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="728" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="728" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A728" s="3">
         <v>749</v>
       </c>
@@ -27525,7 +28381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="729" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="729" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A729" s="3">
         <v>750</v>
       </c>
@@ -27554,7 +28410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="730" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="730" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A730" s="3">
         <v>751</v>
       </c>
@@ -27583,7 +28439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="731" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="731" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A731" s="3">
         <v>752</v>
       </c>
@@ -27612,7 +28468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="732" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="732" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A732" s="3">
         <v>753</v>
       </c>
@@ -27641,7 +28497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="733" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="733" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A733" s="3">
         <v>754</v>
       </c>
@@ -27670,7 +28526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="734" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="734" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A734" s="3">
         <v>755</v>
       </c>
@@ -27699,7 +28555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="735" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="735" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A735" s="3">
         <v>756</v>
       </c>
@@ -27727,8 +28583,23 @@
       <c r="I735" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="736" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J735" s="4">
+        <v>0</v>
+      </c>
+      <c r="K735" s="4">
+        <v>1</v>
+      </c>
+      <c r="L735" s="4">
+        <v>1</v>
+      </c>
+      <c r="M735" s="4">
+        <v>0</v>
+      </c>
+      <c r="N735" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="736" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A736" s="3">
         <v>757</v>
       </c>
@@ -30077,7 +30948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="817" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="817" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A817" s="3">
         <v>839</v>
       </c>
@@ -30106,7 +30977,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="818" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="818" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A818" s="3">
         <v>840</v>
       </c>
@@ -30135,7 +31006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="819" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="819" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A819" s="3">
         <v>841</v>
       </c>
@@ -30164,7 +31035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="820" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="820" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A820" s="3">
         <v>842</v>
       </c>
@@ -30193,7 +31064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="821" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="821" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A821" s="3">
         <v>843</v>
       </c>
@@ -30222,7 +31093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="822" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="822" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A822" s="3">
         <v>844</v>
       </c>
@@ -30251,7 +31122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="823" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="823" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A823" s="3">
         <v>845</v>
       </c>
@@ -30280,7 +31151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="824" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="824" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A824" s="3">
         <v>846</v>
       </c>
@@ -30308,8 +31179,26 @@
       <c r="I824" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="825" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J824" s="4">
+        <v>0</v>
+      </c>
+      <c r="K824" s="4">
+        <v>0</v>
+      </c>
+      <c r="L824" s="4">
+        <v>1</v>
+      </c>
+      <c r="M824" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N824" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O824" s="4" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="825" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A825" s="3">
         <v>847</v>
       </c>
@@ -30338,7 +31227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="826" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="826" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A826" s="3">
         <v>848</v>
       </c>
@@ -30367,7 +31256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="827" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="827" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A827" s="3">
         <v>849</v>
       </c>
@@ -30396,7 +31285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="828" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="828" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A828" s="3">
         <v>850</v>
       </c>
@@ -30425,7 +31314,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="829" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="829" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A829" s="3">
         <v>851</v>
       </c>
@@ -30454,7 +31343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="830" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="830" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A830" s="3">
         <v>853</v>
       </c>
@@ -30482,8 +31371,26 @@
       <c r="I830" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="831" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J830" s="4">
+        <v>0</v>
+      </c>
+      <c r="K830" s="4">
+        <v>0</v>
+      </c>
+      <c r="L830" s="4">
+        <v>1</v>
+      </c>
+      <c r="M830" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N830" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O830" s="4" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="831" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A831" s="3">
         <v>854</v>
       </c>
@@ -30512,7 +31419,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="832" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="832" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A832" s="3">
         <v>855</v>
       </c>
@@ -30541,7 +31448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="833" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="833" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A833" s="3">
         <v>856</v>
       </c>
@@ -30569,8 +31476,26 @@
       <c r="I833" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="834" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J833" s="4">
+        <v>0</v>
+      </c>
+      <c r="K833" s="4">
+        <v>0</v>
+      </c>
+      <c r="L833" s="4">
+        <v>1</v>
+      </c>
+      <c r="M833" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N833" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O833" s="4" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="834" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A834" s="3">
         <v>857</v>
       </c>
@@ -30599,7 +31524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="835" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="835" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A835" s="3">
         <v>858</v>
       </c>
@@ -30628,7 +31553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="836" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="836" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A836" s="3">
         <v>859</v>
       </c>
@@ -30657,7 +31582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="837" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="837" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A837" s="3">
         <v>860</v>
       </c>
@@ -30685,8 +31610,26 @@
       <c r="I837" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="838" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J837" s="4">
+        <v>0</v>
+      </c>
+      <c r="K837" s="4">
+        <v>0</v>
+      </c>
+      <c r="L837" s="4">
+        <v>1</v>
+      </c>
+      <c r="M837" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N837" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O837" s="4" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="838" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A838" s="3">
         <v>861</v>
       </c>
@@ -30715,7 +31658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="839" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="839" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A839" s="3">
         <v>862</v>
       </c>
@@ -30744,7 +31687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="840" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="840" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A840" s="3">
         <v>863</v>
       </c>
@@ -30773,7 +31716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="841" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="841" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A841" s="3">
         <v>864</v>
       </c>
@@ -30802,7 +31745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="842" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="842" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A842" s="3">
         <v>865</v>
       </c>
@@ -30831,7 +31774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="843" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="843" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A843" s="3">
         <v>866</v>
       </c>
@@ -30860,7 +31803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="844" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="844" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A844" s="3">
         <v>867</v>
       </c>
@@ -30889,7 +31832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="845" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="845" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A845" s="3">
         <v>868</v>
       </c>
@@ -30918,7 +31861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="846" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="846" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A846" s="3">
         <v>869</v>
       </c>
@@ -30947,7 +31890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="847" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="847" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A847" s="3">
         <v>870</v>
       </c>
@@ -30976,7 +31919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="848" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="848" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A848" s="3">
         <v>871</v>
       </c>

</xml_diff>

<commit_message>
Error check for sparrow meeting
</commit_message>
<xml_diff>
--- a/R_VisualizeOldMethods.xlsx
+++ b/R_VisualizeOldMethods.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4685" uniqueCount="1563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4686" uniqueCount="1563">
   <si>
     <t>DVDRef</t>
   </si>
@@ -5593,9 +5593,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1528"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I694" sqref="I694"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A807" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O815" sqref="O815"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30484,7 +30484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="801" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="801" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A801" s="3">
         <v>823</v>
       </c>
@@ -30513,7 +30513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="802" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="802" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A802" s="3">
         <v>824</v>
       </c>
@@ -30542,7 +30542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="803" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="803" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A803" s="3">
         <v>825</v>
       </c>
@@ -30571,7 +30571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="804" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="804" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A804" s="3">
         <v>826</v>
       </c>
@@ -30600,7 +30600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="805" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="805" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A805" s="3">
         <v>827</v>
       </c>
@@ -30629,7 +30629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="806" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="806" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A806" s="3">
         <v>828</v>
       </c>
@@ -30658,7 +30658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="807" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="807" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A807" s="3">
         <v>829</v>
       </c>
@@ -30687,7 +30687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="808" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="808" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A808" s="3">
         <v>830</v>
       </c>
@@ -30716,7 +30716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="809" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="809" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A809" s="3">
         <v>831</v>
       </c>
@@ -30745,7 +30745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="810" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="810" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A810" s="3">
         <v>832</v>
       </c>
@@ -30774,7 +30774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="811" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="811" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A811" s="3">
         <v>833</v>
       </c>
@@ -30803,7 +30803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="812" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="812" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A812" s="3">
         <v>834</v>
       </c>
@@ -30832,7 +30832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="813" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="813" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A813" s="3">
         <v>835</v>
       </c>
@@ -30861,7 +30861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="814" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="814" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A814" s="3">
         <v>836</v>
       </c>
@@ -30890,7 +30890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="815" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="815" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A815" s="3">
         <v>837</v>
       </c>
@@ -30918,8 +30918,26 @@
       <c r="I815" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="816" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J815" s="4">
+        <v>1</v>
+      </c>
+      <c r="K815" s="4">
+        <v>0</v>
+      </c>
+      <c r="L815" s="4">
+        <v>1</v>
+      </c>
+      <c r="M815" s="4">
+        <v>0</v>
+      </c>
+      <c r="N815" s="4">
+        <v>0</v>
+      </c>
+      <c r="O815" s="4" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="816" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A816" s="3">
         <v>838</v>
       </c>

</xml_diff>

<commit_message>
last changes in excel files done !
</commit_message>
<xml_diff>
--- a/R_VisualizeOldMethods.xlsx
+++ b/R_VisualizeOldMethods.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4693" uniqueCount="1568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4695" uniqueCount="1569">
   <si>
     <t>DVDRef</t>
   </si>
@@ -4718,6 +4718,9 @@
   </si>
   <si>
     <t>one O grey might be a stay ?</t>
+  </si>
+  <si>
+    <t>added grey to 'O'. Could see from video that 'S' time not written done</t>
   </si>
 </sst>
 </file>
@@ -5608,9 +5611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1530"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O382" sqref="O382"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A719" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O731" sqref="O731"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28173,7 +28176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="721" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="721" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A721" s="3">
         <v>741</v>
       </c>
@@ -28202,7 +28205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="722" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="722" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A722" s="3">
         <v>742</v>
       </c>
@@ -28231,7 +28234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="723" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="723" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A723" s="3">
         <v>743</v>
       </c>
@@ -28260,7 +28263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="724" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="724" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A724" s="3">
         <v>744</v>
       </c>
@@ -28289,7 +28292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="725" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="725" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A725" s="3">
         <v>745</v>
       </c>
@@ -28318,7 +28321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="726" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="726" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A726" s="3">
         <v>746</v>
       </c>
@@ -28346,8 +28349,26 @@
       <c r="I726" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="727" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J726" s="4">
+        <v>0</v>
+      </c>
+      <c r="K726" s="4">
+        <v>1</v>
+      </c>
+      <c r="L726" s="4">
+        <v>1</v>
+      </c>
+      <c r="M726" s="4">
+        <v>0</v>
+      </c>
+      <c r="N726" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O726" s="4" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="727" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A727" s="3">
         <v>747</v>
       </c>
@@ -28376,7 +28397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="728" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="728" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A728" s="3">
         <v>748</v>
       </c>
@@ -28405,7 +28426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="729" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="729" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A729" s="3">
         <v>749</v>
       </c>
@@ -28434,7 +28455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="730" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="730" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A730" s="3">
         <v>750</v>
       </c>
@@ -28463,7 +28484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="731" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="731" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A731" s="3">
         <v>751</v>
       </c>
@@ -28492,7 +28513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="732" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="732" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A732" s="3">
         <v>752</v>
       </c>
@@ -28521,7 +28542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="733" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="733" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A733" s="3">
         <v>753</v>
       </c>
@@ -28550,7 +28571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="734" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="734" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A734" s="3">
         <v>754</v>
       </c>
@@ -28579,7 +28600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="735" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="735" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A735" s="3">
         <v>755</v>
       </c>
@@ -28608,7 +28629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="736" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="736" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A736" s="3">
         <v>756</v>
       </c>

</xml_diff>